<commit_message>
7th commit Test Cases Added
</commit_message>
<xml_diff>
--- a/testdata/testData_mirror.xlsx
+++ b/testdata/testData_mirror.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="18" r:id="rId1"/>
@@ -13,8 +13,8 @@
     <sheet name="tc_001" sheetId="19" r:id="rId4"/>
     <sheet name="tc_002" sheetId="20" r:id="rId5"/>
     <sheet name="tc_003" sheetId="21" r:id="rId6"/>
-    <sheet name="tc_005" sheetId="25" r:id="rId7"/>
-    <sheet name="tc_016" sheetId="26" r:id="rId8"/>
+    <sheet name="tc_006" sheetId="25" r:id="rId7"/>
+    <sheet name="tc_007" sheetId="26" r:id="rId8"/>
     <sheet name="tc_004" sheetId="24" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -791,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -828,7 +828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
9th commit Test Cases Updated
</commit_message>
<xml_diff>
--- a/testdata/testData_mirror.xlsx
+++ b/testdata/testData_mirror.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="18" r:id="rId1"/>
@@ -14,15 +14,16 @@
     <sheet name="tc_002" sheetId="20" r:id="rId5"/>
     <sheet name="tc_003" sheetId="21" r:id="rId6"/>
     <sheet name="tc_006" sheetId="25" r:id="rId7"/>
-    <sheet name="tc_007" sheetId="26" r:id="rId8"/>
-    <sheet name="tc_004" sheetId="24" r:id="rId9"/>
+    <sheet name="tc_009" sheetId="27" r:id="rId8"/>
+    <sheet name="tc_007" sheetId="26" r:id="rId9"/>
+    <sheet name="tc_004" sheetId="24" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>Passoword</t>
   </si>
@@ -112,6 +113,9 @@
   </si>
   <si>
     <t>upload_test_automation.a2l</t>
+  </si>
+  <si>
+    <t>Test A2L Data</t>
   </si>
 </sst>
 </file>
@@ -546,6 +550,18 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
@@ -791,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -825,6 +841,36 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -858,16 +904,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
11th commit Test Cases Updated
</commit_message>
<xml_diff>
--- a/testdata/testData_mirror.xlsx
+++ b/testdata/testData_mirror.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>Passoword</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Test A2L Data</t>
+  </si>
+  <si>
+    <t>a2l_file_name/comment</t>
   </si>
 </sst>
 </file>
@@ -845,7 +848,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -855,7 +858,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B1" s="4"/>
     </row>

</xml_diff>

<commit_message>
13th commit Test Cases Added
</commit_message>
<xml_diff>
--- a/testdata/testData_mirror.xlsx
+++ b/testdata/testData_mirror.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="18" r:id="rId1"/>
@@ -15,15 +15,16 @@
     <sheet name="tc_003" sheetId="21" r:id="rId6"/>
     <sheet name="tc_006" sheetId="25" r:id="rId7"/>
     <sheet name="tc_009" sheetId="27" r:id="rId8"/>
-    <sheet name="tc_007" sheetId="26" r:id="rId9"/>
-    <sheet name="tc_004" sheetId="24" r:id="rId10"/>
+    <sheet name="tc_018" sheetId="28" r:id="rId9"/>
+    <sheet name="tc_007" sheetId="26" r:id="rId10"/>
+    <sheet name="tc_004" sheetId="24" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>Passoword</t>
   </si>
@@ -119,6 +120,18 @@
   </si>
   <si>
     <t>a2l_file_name/comment</t>
+  </si>
+  <si>
+    <t>Release letter comment automation test</t>
+  </si>
+  <si>
+    <t>Release letter comment</t>
+  </si>
+  <si>
+    <t>Internal comment automation test</t>
+  </si>
+  <si>
+    <t>Internal Comment</t>
   </si>
 </sst>
 </file>
@@ -555,6 +568,42 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -847,7 +896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -875,36 +924,37 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>29</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C2" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
20th commit Test Cases Updated
</commit_message>
<xml_diff>
--- a/testdata/testData_mirror.xlsx
+++ b/testdata/testData_mirror.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="18" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>Passoword</t>
   </si>
@@ -32,106 +32,112 @@
     <t>Username</t>
   </si>
   <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>V7 Test</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>V8 Release Date(mm/dd/yyyy)</t>
+  </si>
+  <si>
+    <t>V8</t>
+  </si>
+  <si>
+    <t>ANAVINA</t>
+  </si>
+  <si>
+    <t>V7 Description Test</t>
+  </si>
+  <si>
+    <t>V4..V8 Admin</t>
+  </si>
+  <si>
+    <t>Application Name</t>
+  </si>
+  <si>
+    <t>12/08/2021</t>
+  </si>
+  <si>
+    <t>Avinash Ankush [ANAVINA]</t>
+  </si>
+  <si>
+    <t>Project Write Access</t>
+  </si>
+  <si>
+    <t>Care Group</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>Care_AKV Varient</t>
+  </si>
+  <si>
+    <t>TEST AKV Variant _kraoliv_</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Test automation Release Update</t>
+  </si>
+  <si>
+    <t>12/12/2021</t>
+  </si>
+  <si>
+    <t>Release created for test automation validation</t>
+  </si>
+  <si>
+    <t>Test Automation Release</t>
+  </si>
+  <si>
+    <t>Release updated for test automation validation</t>
+  </si>
+  <si>
+    <t>Sahoo Sukriti [suksaho]</t>
+  </si>
+  <si>
+    <t>Upload created by Test Automation</t>
+  </si>
+  <si>
+    <t>a2l_file_name</t>
+  </si>
+  <si>
+    <t>upload_test_automation.a2l</t>
+  </si>
+  <si>
+    <t>Test A2L Data</t>
+  </si>
+  <si>
+    <t>a2l_file_name/comment</t>
+  </si>
+  <si>
+    <t>Release letter comment automation test</t>
+  </si>
+  <si>
+    <t>Release letter comment</t>
+  </si>
+  <si>
+    <t>Internal comment automation test</t>
+  </si>
+  <si>
+    <t>Internal Comment</t>
+  </si>
+  <si>
     <t>anavina</t>
   </si>
   <si>
     <t>Password@12345</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>V7 Test</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>V8 Release Date(mm/dd/yyyy)</t>
-  </si>
-  <si>
-    <t>V8</t>
-  </si>
-  <si>
-    <t>ANAVINA</t>
-  </si>
-  <si>
-    <t>V7 Description Test</t>
-  </si>
-  <si>
-    <t>V4..V8 Admin</t>
-  </si>
-  <si>
-    <t>Application Name</t>
-  </si>
-  <si>
-    <t>12/08/2021</t>
-  </si>
-  <si>
-    <t>Avinash Ankush [ANAVINA]</t>
-  </si>
-  <si>
-    <t>Project Write Access</t>
-  </si>
-  <si>
-    <t>Care Group</t>
-  </si>
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>Care_AKV Varient</t>
-  </si>
-  <si>
-    <t>TEST AKV Variant _kraoliv_</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Test automation Release Update</t>
-  </si>
-  <si>
-    <t>12/12/2021</t>
-  </si>
-  <si>
-    <t>Release created for test automation validation</t>
-  </si>
-  <si>
-    <t>Test Automation Release</t>
-  </si>
-  <si>
-    <t>Release updated for test automation validation</t>
-  </si>
-  <si>
-    <t>Sahoo Sukriti [suksaho]</t>
-  </si>
-  <si>
-    <t>Upload created by Test Automation</t>
-  </si>
-  <si>
-    <t>a2l_file_name</t>
-  </si>
-  <si>
-    <t>upload_test_automation.a2l</t>
-  </si>
-  <si>
-    <t>Test A2L Data</t>
-  </si>
-  <si>
-    <t>a2l_file_name/comment</t>
-  </si>
-  <si>
-    <t>Release letter comment automation test</t>
-  </si>
-  <si>
-    <t>Release letter comment</t>
-  </si>
-  <si>
-    <t>Internal comment automation test</t>
-  </si>
-  <si>
-    <t>Internal Comment</t>
+    <t>automation_user</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -531,9 +537,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -549,17 +557,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -582,18 +598,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -629,12 +645,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -660,37 +676,37 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F2" s="5"/>
     </row>
@@ -720,13 +736,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="C1" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -734,10 +750,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -766,29 +782,29 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E2" s="5"/>
     </row>
@@ -815,37 +831,37 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F2" s="5"/>
     </row>
@@ -871,19 +887,19 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -907,13 +923,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5"/>
     </row>
@@ -926,7 +942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -938,20 +954,20 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="C2" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
23rd commit Test Cases Updated
</commit_message>
<xml_diff>
--- a/testdata/testData_mirror.xlsx
+++ b/testdata/testData_mirror.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="18" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
   <si>
     <t>Passoword</t>
   </si>
@@ -77,18 +77,12 @@
     <t>Care_AKV Varient</t>
   </si>
   <si>
-    <t>TEST AKV Variant _kraoliv_</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
     <t>Test automation Release Update</t>
   </si>
   <si>
-    <t>12/12/2021</t>
-  </si>
-  <si>
     <t>Release created for test automation validation</t>
   </si>
   <si>
@@ -128,16 +122,52 @@
     <t>Internal Comment</t>
   </si>
   <si>
-    <t>anavina</t>
-  </si>
-  <si>
-    <t>Password@12345</t>
-  </si>
-  <si>
-    <t>automation_user</t>
-  </si>
-  <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>v7_automation_user</t>
+  </si>
+  <si>
+    <t>User Type</t>
+  </si>
+  <si>
+    <t>normal user</t>
+  </si>
+  <si>
+    <t>v4 user</t>
+  </si>
+  <si>
+    <t>v7_automation_v4_user</t>
+  </si>
+  <si>
+    <t>v5 user</t>
+  </si>
+  <si>
+    <t>v7_automation_v5_user</t>
+  </si>
+  <si>
+    <t>v6 user</t>
+  </si>
+  <si>
+    <t>v7_automation_v6_user</t>
+  </si>
+  <si>
+    <t>v7 user</t>
+  </si>
+  <si>
+    <t>v7_automation_v7_user</t>
+  </si>
+  <si>
+    <t>v8 user</t>
+  </si>
+  <si>
+    <t>v7_automation_v8_user</t>
+  </si>
+  <si>
+    <t>v7_care_akv_variant_automation_test</t>
+  </si>
+  <si>
+    <t>27/01/2022</t>
   </si>
 </sst>
 </file>
@@ -217,7 +247,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -232,6 +262,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -537,48 +568,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.7265625" customWidth="1"/>
     <col min="2" max="2" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>35</v>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -598,18 +680,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -694,10 +776,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>11</v>
@@ -770,14 +852,14 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" customWidth="1"/>
-    <col min="3" max="3" width="22.6328125" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -817,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -849,19 +931,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F2" s="5"/>
     </row>
@@ -876,13 +958,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -899,7 +981,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -923,13 +1005,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="5"/>
     </row>
@@ -954,19 +1036,19 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="C2" s="5"/>
     </row>

</xml_diff>

<commit_message>
24th commit Final 001-014 Updated
</commit_message>
<xml_diff>
--- a/testdata/testData_mirror.xlsx
+++ b/testdata/testData_mirror.xlsx
@@ -4,20 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="18" r:id="rId1"/>
-    <sheet name="Dashboard" sheetId="23" r:id="rId2"/>
-    <sheet name="Basic_Information_Release" sheetId="22" r:id="rId3"/>
+    <sheet name="Basic_Information_Release" sheetId="22" r:id="rId2"/>
+    <sheet name="Dashboard" sheetId="23" r:id="rId3"/>
     <sheet name="tc_001" sheetId="19" r:id="rId4"/>
     <sheet name="tc_002" sheetId="20" r:id="rId5"/>
     <sheet name="tc_003" sheetId="21" r:id="rId6"/>
-    <sheet name="tc_006" sheetId="25" r:id="rId7"/>
-    <sheet name="tc_009" sheetId="27" r:id="rId8"/>
-    <sheet name="tc_018" sheetId="28" r:id="rId9"/>
-    <sheet name="tc_007" sheetId="26" r:id="rId10"/>
-    <sheet name="tc_004" sheetId="24" r:id="rId11"/>
+    <sheet name="tc_008" sheetId="25" r:id="rId7"/>
+    <sheet name="tc_009" sheetId="26" r:id="rId8"/>
+    <sheet name="tc_011" sheetId="27" r:id="rId9"/>
+    <sheet name="tc_004" sheetId="28" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -83,6 +82,9 @@
     <t>Test automation Release Update</t>
   </si>
   <si>
+    <t>12/12/2021</t>
+  </si>
+  <si>
     <t>Release created for test automation validation</t>
   </si>
   <si>
@@ -104,9 +106,6 @@
     <t>upload_test_automation.a2l</t>
   </si>
   <si>
-    <t>Test A2L Data</t>
-  </si>
-  <si>
     <t>a2l_file_name/comment</t>
   </si>
   <si>
@@ -122,18 +121,18 @@
     <t>Internal Comment</t>
   </si>
   <si>
+    <t>User Type</t>
+  </si>
+  <si>
+    <t>normal user</t>
+  </si>
+  <si>
+    <t>v7_automation_user</t>
+  </si>
+  <si>
     <t>test</t>
   </si>
   <si>
-    <t>v7_automation_user</t>
-  </si>
-  <si>
-    <t>User Type</t>
-  </si>
-  <si>
-    <t>normal user</t>
-  </si>
-  <si>
     <t>v4 user</t>
   </si>
   <si>
@@ -167,14 +166,14 @@
     <t>v7_care_akv_variant_automation_test</t>
   </si>
   <si>
-    <t>27/01/2022</t>
+    <t>v7_automation_with_q_group</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,23 +182,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -243,29 +234,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -571,47 +554,47 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7265625" customWidth="1"/>
+    <col min="1" max="1" width="17.6328125" customWidth="1"/>
     <col min="2" max="2" width="25.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -622,7 +605,7 @@
         <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -633,7 +616,7 @@
         <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -644,7 +627,7 @@
         <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -655,7 +638,7 @@
         <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -666,53 +649,102 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>25</v>
-      </c>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="28.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="23.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D4" s="4"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -734,66 +766,6 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="28.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="23.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D4" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -817,30 +789,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -852,43 +824,43 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" customWidth="1"/>
+    <col min="3" max="3" width="22.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="E2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -899,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -912,40 +884,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="4"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -968,22 +940,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="4"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -995,62 +967,61 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="4"/>
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="4"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="5"/>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
25th commit Final 001-017 Updated
</commit_message>
<xml_diff>
--- a/testdata/testData_mirror.xlsx
+++ b/testdata/testData_mirror.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="18" r:id="rId1"/>
@@ -94,9 +94,6 @@
     <t>Release updated for test automation validation</t>
   </si>
   <si>
-    <t>Sahoo Sukriti [suksaho]</t>
-  </si>
-  <si>
     <t>Upload created by Test Automation</t>
   </si>
   <si>
@@ -167,6 +164,9 @@
   </si>
   <si>
     <t>v7_automation_with_q_group</t>
+  </si>
+  <si>
+    <t>v7_automation_v8_user [v7_automation_v8_user]</t>
   </si>
 </sst>
 </file>
@@ -566,7 +566,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -577,68 +577,68 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
         <v>38</v>
       </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
         <v>40</v>
       </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
         <v>42</v>
       </c>
-      <c r="B6" t="s">
-        <v>43</v>
-      </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
         <v>44</v>
       </c>
-      <c r="B7" t="s">
-        <v>45</v>
-      </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -651,7 +651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -663,19 +663,19 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -689,7 +689,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -697,7 +697,8 @@
     <col min="1" max="1" width="28.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.90625" customWidth="1"/>
+    <col min="5" max="5" width="23.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -729,7 +730,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>12</v>
@@ -871,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -912,10 +913,10 @@
         <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F2" s="3"/>
     </row>
@@ -953,7 +954,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -981,15 +982,15 @@
         <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1013,13 +1014,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3"/>
     </row>

</xml_diff>

<commit_message>
28th commit Final 001-019 Updated
</commit_message>
<xml_diff>
--- a/testdata/testData_mirror.xlsx
+++ b/testdata/testData_mirror.xlsx
@@ -693,7 +693,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1812389</t>
+          <t>1819117</t>
         </is>
       </c>
     </row>
@@ -705,7 +705,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1812442</t>
+          <t>1819118</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
30th commit Final 001-019 Updated
</commit_message>
<xml_diff>
--- a/testdata/testData_mirror.xlsx
+++ b/testdata/testData_mirror.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" firstSheet="0" activeTab="10" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,10 +12,10 @@
     <sheet name="tc_001" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="tc_002" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="tc_003" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="tc_008" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="tc_009" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="tc_011" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="tc_004" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="tc_004" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="tc_008" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="tc_009" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="tc_011" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="release_id" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
@@ -612,43 +612,32 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col width="34.7265625" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="29.90625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="26.453125" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>Release letter comment</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>Internal Comment</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="n"/>
+          <t>a2l_file_name/comment</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>Release letter comment automation test</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>Internal comment automation test</t>
-        </is>
-      </c>
-      <c r="C2" s="3" t="n"/>
+          <t>v7_automation_with_q_group</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -663,7 +652,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -693,7 +682,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1819168</t>
+          <t>1823223</t>
         </is>
       </c>
     </row>
@@ -705,7 +694,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1819191</t>
+          <t>1819214</t>
         </is>
       </c>
     </row>
@@ -722,8 +711,8 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -776,7 +765,7 @@
       </c>
       <c r="C2" s="5" t="inlineStr">
         <is>
-          <t>12/08/2021</t>
+          <t>01/26/2022</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
@@ -844,7 +833,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:F2"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -905,7 +894,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:D2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -1053,6 +1042,55 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <cols>
+    <col width="34.7265625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="29.90625" bestFit="1" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Release letter comment</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Internal Comment</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>Release letter comment automation test</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>Internal comment automation test</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1093,7 +1131,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1139,42 +1177,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
-  <cols>
-    <col width="26.453125" bestFit="1" customWidth="1" min="1" max="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>a2l_file_name/comment</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="n"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>v7_automation_with_q_group</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="n"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
39th commit Final 001-047
</commit_message>
<xml_diff>
--- a/testdata/testData_mirror.xlsx
+++ b/testdata/testData_mirror.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
   <si>
     <t>User Type</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>v7_akv_variant_automation_test</t>
+  </si>
+  <si>
+    <t>v7_automation_v8_user [v7_automation_v8_user]</t>
   </si>
 </sst>
 </file>
@@ -684,7 +687,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -692,7 +695,7 @@
     <col min="1" max="1" width="28.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.54296875" customWidth="1"/>
     <col min="5" max="5" width="23.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -725,7 +728,7 @@
         <v>23</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
40th commit Final 001-048
</commit_message>
<xml_diff>
--- a/testdata/testData_mirror.xlsx
+++ b/testdata/testData_mirror.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,14 @@
     <sheet name="tc_008" sheetId="8" r:id="rId8"/>
     <sheet name="tc_009" sheetId="9" r:id="rId9"/>
     <sheet name="tc_011" sheetId="10" r:id="rId10"/>
+    <sheet name="tc_047" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>User Type</t>
   </si>
@@ -172,6 +173,12 @@
   </si>
   <si>
     <t>v7_automation_v8_user [v7_automation_v8_user]</t>
+  </si>
+  <si>
+    <t>reject_comment_v4_user</t>
+  </si>
+  <si>
+    <t>Reject comment as V4 user automation test</t>
   </si>
 </sst>
 </file>
@@ -682,11 +689,39 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="41.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -776,7 +811,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
41st commit Final 001-050
</commit_message>
<xml_diff>
--- a/testdata/testData_mirror.xlsx
+++ b/testdata/testData_mirror.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -23,13 +23,14 @@
     <sheet name="tc_009" sheetId="9" r:id="rId9"/>
     <sheet name="tc_011" sheetId="10" r:id="rId10"/>
     <sheet name="tc_047" sheetId="11" r:id="rId11"/>
+    <sheet name="tc_049" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
   <si>
     <t>User Type</t>
   </si>
@@ -179,6 +180,12 @@
   </si>
   <si>
     <t>Reject comment as V4 user automation test</t>
+  </si>
+  <si>
+    <t>reject_comment_v5_user</t>
+  </si>
+  <si>
+    <t>Reject comment as V5 user automation test</t>
   </si>
 </sst>
 </file>
@@ -693,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -710,6 +717,34 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="37.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
43rd commit Final 001-041
</commit_message>
<xml_diff>
--- a/testdata/testData_mirror.xlsx
+++ b/testdata/testData_mirror.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" activeTab="12"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" firstSheet="1" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,14 @@
     <sheet name="tc_047" sheetId="11" r:id="rId11"/>
     <sheet name="tc_049" sheetId="12" r:id="rId12"/>
     <sheet name="tc_051" sheetId="13" r:id="rId13"/>
+    <sheet name="tc_053" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
   <si>
     <t>User Type</t>
   </si>
@@ -193,6 +194,12 @@
   </si>
   <si>
     <t>Reject comment as V6 user automation test</t>
+  </si>
+  <si>
+    <t>reject_comment_v7_user</t>
+  </si>
+  <si>
+    <t>Reject comment as V7 user automation test</t>
   </si>
 </sst>
 </file>
@@ -763,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -780,6 +787,34 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="37.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
45th commit Final 001-055
</commit_message>
<xml_diff>
--- a/testdata/testData_mirror.xlsx
+++ b/testdata/testData_mirror.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" firstSheet="1" activeTab="13"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
   <si>
     <t>User Type</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>Reject comment as V7 user automation test</t>
+  </si>
+  <si>
+    <t>v7_akv_without_q_automation_test</t>
   </si>
 </sst>
 </file>
@@ -798,7 +801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1103,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1133,6 +1136,11 @@
       </c>
       <c r="C2" s="3"/>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
46th commit Final 001-047
</commit_message>
<xml_diff>
--- a/testdata/testData_mirror.xlsx
+++ b/testdata/testData_mirror.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" firstSheet="2" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -26,13 +26,14 @@
     <sheet name="tc_049" sheetId="12" r:id="rId12"/>
     <sheet name="tc_051" sheetId="13" r:id="rId13"/>
     <sheet name="tc_053" sheetId="14" r:id="rId14"/>
+    <sheet name="tc_056" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
   <si>
     <t>User Type</t>
   </si>
@@ -203,6 +204,9 @@
   </si>
   <si>
     <t>v7_akv_without_q_automation_test</t>
+  </si>
+  <si>
+    <t>without_q_group_test</t>
   </si>
 </sst>
 </file>
@@ -688,7 +692,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -818,6 +822,48 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1106,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1136,11 +1182,6 @@
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
56th commit Final 001-056
</commit_message>
<xml_diff>
--- a/testdata/testData_mirror.xlsx
+++ b/testdata/testData_mirror.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" firstSheet="2" activeTab="14"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" firstSheet="2" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -27,13 +27,14 @@
     <sheet name="tc_051" sheetId="13" r:id="rId13"/>
     <sheet name="tc_053" sheetId="14" r:id="rId14"/>
     <sheet name="tc_056" sheetId="15" r:id="rId15"/>
+    <sheet name="tc_058" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
   <si>
     <t>User Type</t>
   </si>
@@ -207,13 +208,25 @@
   </si>
   <si>
     <t>without_q_group_test</t>
+  </si>
+  <si>
+    <t>admin user</t>
+  </si>
+  <si>
+    <t>anavina</t>
+  </si>
+  <si>
+    <t>admin password</t>
+  </si>
+  <si>
+    <t>Password@12345</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +244,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -274,10 +295,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -287,8 +309,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -714,6 +738,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -742,6 +767,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -770,6 +796,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -798,6 +825,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -826,6 +854,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -833,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -868,6 +897,49 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -929,6 +1001,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -957,6 +1030,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1004,6 +1078,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1052,6 +1127,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1147,6 +1223,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1184,6 +1261,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
58th commit Final 001-058
</commit_message>
<xml_diff>
--- a/testdata/testData_mirror.xlsx
+++ b/testdata/testData_mirror.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="828" firstSheet="2" activeTab="15"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="769" firstSheet="7" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -28,13 +28,14 @@
     <sheet name="tc_053" sheetId="14" r:id="rId14"/>
     <sheet name="tc_056" sheetId="15" r:id="rId15"/>
     <sheet name="tc_058" sheetId="16" r:id="rId16"/>
+    <sheet name="tc_064" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="70">
   <si>
     <t>User Type</t>
   </si>
@@ -220,13 +221,37 @@
   </si>
   <si>
     <t>Password@12345</t>
+  </si>
+  <si>
+    <t>v4 primary user</t>
+  </si>
+  <si>
+    <t>v5 primary user</t>
+  </si>
+  <si>
+    <t>v6 primary user</t>
+  </si>
+  <si>
+    <t>v7 primary user</t>
+  </si>
+  <si>
+    <t>v4 fallback user</t>
+  </si>
+  <si>
+    <t>v5 fallback user</t>
+  </si>
+  <si>
+    <t>v6 fallback user</t>
+  </si>
+  <si>
+    <t>v7 fallback user</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,6 +277,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -299,7 +331,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -310,6 +342,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -707,7 +742,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K007a93Internal&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -739,6 +777,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K007a93Internal&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -768,6 +809,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K007a93Internal&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -797,6 +841,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K007a93Internal&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -826,6 +873,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K007a93Internal&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -855,6 +905,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K007a93Internal&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -898,41 +951,97 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K007a93Internal&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="18.6328125" customWidth="1"/>
+    <col min="5" max="5" width="19.1796875" customWidth="1"/>
+    <col min="6" max="6" width="19.08984375" customWidth="1"/>
+    <col min="7" max="7" width="18.7265625" customWidth="1"/>
+    <col min="8" max="8" width="19.54296875" customWidth="1"/>
+    <col min="9" max="9" width="19.08984375" customWidth="1"/>
+    <col min="10" max="10" width="18.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -940,6 +1049,41 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K007a93Internal&amp;1#</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="37.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K007a93Internal&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1002,6 +1146,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K007a93Internal&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1031,6 +1178,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K007a93Internal&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1079,6 +1229,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K007a93Internal&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1128,6 +1281,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K007a93Internal&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1185,7 +1341,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K007a93Internal&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1224,6 +1383,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K007a93Internal&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1262,6 +1424,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K007a93Internal&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1297,6 +1462,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K007a93Internal&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>